<commit_message>
Updated plans and inventory
</commit_message>
<xml_diff>
--- a/Finances/Inventory/Inventory.xlsx
+++ b/Finances/Inventory/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="149">
   <si>
     <t>Item</t>
   </si>
@@ -315,9 +315,6 @@
     <t>Camel Divider</t>
   </si>
   <si>
-    <t>Camel Metal Compass</t>
-  </si>
-  <si>
     <t>Camel 150mm Ruler</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>3M Scotch 35 White Vinyl Electrical Tape 3/4" Wide</t>
   </si>
   <si>
-    <t>IPG 1 3/8" Masking Tape</t>
-  </si>
-  <si>
     <t>Meccano Erector Super Construction Set 25-in-1 Reference #: 837080</t>
   </si>
   <si>
@@ -432,10 +426,46 @@
     <t>Foundation 1 Foundation 2 Test Bed</t>
   </si>
   <si>
-    <t>Paper Washers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Note: Some construction materials are packaged products that contain other construction materials. Parts are not mentioned. These may be mentioned and used in instructions during assembly. For example, nuts and bolts kit will contain various nuts and various bolts. To list each item in the kit in iventory would be inordinate, so the product code for that kit and its name are listed. </t>
+  </si>
+  <si>
+    <t>Titebond III Ultimate Wood Glue Waterproof Exterior/Interior 16 FL. OZ.</t>
+  </si>
+  <si>
+    <t>40+</t>
+  </si>
+  <si>
+    <t>Paper Mate Clearpoint Mechanical Pencils 0.7mm HB #2</t>
+  </si>
+  <si>
+    <t>Paper Mate 0.7mm HB #2 Lead Refills</t>
+  </si>
+  <si>
+    <t>Replacement Needed</t>
+  </si>
+  <si>
+    <t>Camel Metal Compass with Pencil Lock</t>
+  </si>
+  <si>
+    <t>Fiskars 12-96807097 12-Inch/30CM Rotary Paper Trimmer</t>
+  </si>
+  <si>
+    <t>Bamboo Skewers 12"</t>
+  </si>
+  <si>
+    <t>Pushp Captain Bright Electro Nickel Plated M.S. Pins</t>
+  </si>
+  <si>
+    <t>50+</t>
+  </si>
+  <si>
+    <t>IPG 505 Masking Tape 1 3/8"</t>
+  </si>
+  <si>
+    <t>5+</t>
+  </si>
+  <si>
+    <t>Construction Paper Washers 1/4" x 5/8" x 3/8"</t>
   </si>
 </sst>
 </file>
@@ -465,7 +495,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +555,18 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -579,7 +621,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -590,8 +632,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,16 +688,22 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
     <cellStyle name="20% - Accent5" xfId="7" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="10" builtinId="50"/>
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="6" builtinId="40"/>
     <cellStyle name="60% - Accent5" xfId="8" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="11" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="9" builtinId="10"/>
   </cellStyles>
@@ -954,297 +1004,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="71.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="19"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>96</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B16" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B19" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="C19" s="19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B22" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="C22" s="19"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B23" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="C23" s="19"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="19"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B22" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="19"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="19"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B29" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="19"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="19"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="19"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="19"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="19"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="19"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36" s="19"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="19"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B38" s="5">
         <v>2</v>
       </c>
+      <c r="C38" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1473,7 +1588,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -1735,10 +1850,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="14" t="s">
@@ -1747,7 +1862,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B48" s="5">
         <v>5</v>
@@ -1797,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1831,7 +1946,9 @@
       <c r="B2" s="5">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8">
+        <v>5</v>
+      </c>
       <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1841,7 +1958,9 @@
       <c r="B3" s="5">
         <v>8</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8">
+        <v>3</v>
+      </c>
       <c r="D3" s="14" t="s">
         <v>46</v>
       </c>
@@ -1878,21 +1997,23 @@
         <v>46</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="5">
-        <v>69</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>144</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
       <c r="D7" s="14" t="s">
         <v>46</v>
       </c>
@@ -1904,13 +2025,15 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -1919,15 +2042,15 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="5">
-        <v>123</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -1936,13 +2059,17 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="13"/>
+        <v>123</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -1954,12 +2081,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -1968,10 +2093,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
@@ -1985,13 +2110,15 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="5">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -2003,12 +2130,10 @@
         <v>59</v>
       </c>
       <c r="B14" s="5">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="D14" s="13"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -2017,29 +2142,38 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="B15" s="5">
+        <v>18</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="5">
-        <v>22</v>
-      </c>
-      <c r="C16" s="8"/>
+      <c r="B16" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
       <c r="D16" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -2049,7 +2183,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -2059,7 +2193,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="5">
         <v>14</v>
@@ -2071,7 +2205,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>4</v>
@@ -2081,7 +2215,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>4</v>
@@ -2091,87 +2225,93 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="5">
-        <v>200</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="13"/>
+        <v>105</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="12">
-        <v>5</v>
-      </c>
-      <c r="C23" s="8">
-        <v>3</v>
-      </c>
-      <c r="D23" s="13"/>
+        <v>106</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="12">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B24" s="5">
+        <v>200</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B25" s="12">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8">
+        <v>3</v>
+      </c>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="5">
+        <v>65</v>
+      </c>
+      <c r="B26" s="12">
         <v>1</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8"/>
+        <v>136</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
       <c r="D27" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
       <c r="D28" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -2183,7 +2323,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -2195,30 +2335,34 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="B31" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="13"/>
+      <c r="D31" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>5</v>
+        <v>112</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="14" t="s">
@@ -2227,34 +2371,32 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" s="12">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B34" s="5">
+        <v>4</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="12">
-        <v>1</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" s="12">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="B36" s="5">
+        <v>10</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="14" t="s">
@@ -2263,17 +2405,21 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="12">
-        <v>1</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="14"/>
+        <v>66</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="8">
+        <v>16</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -2285,7 +2431,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B39" s="12">
         <v>1</v>
@@ -2297,7 +2443,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B40" s="12">
         <v>1</v>
@@ -2307,9 +2453,61 @@
         <v>46</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="12">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="14"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="12">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
+        <v>1</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" s="12">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F6:J14"/>
+    <mergeCell ref="F6:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2425,7 +2623,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2447,7 +2645,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2458,14 +2656,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2477,7 +2673,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2503,22 +2699,26 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
       <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
       <c r="D3" s="13"/>
     </row>
   </sheetData>

</xml_diff>